<commit_message>
Ajout format indication dans MED et format ano ssr filler ok
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RHA ANO 17.xlsx
+++ b/formats/excel/Formats RHA ANO 17.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$101</definedName>
+  </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
@@ -501,7 +504,7 @@
     <t>PBCMU</t>
   </si>
   <si>
-    <t>FILLER2</t>
+    <t>Filler2</t>
   </si>
   <si>
     <t xml:space="preserve">Identifiant anonyme d'hospitalisation </t>
@@ -528,7 +531,7 @@
     <t>IDHOSPI1</t>
   </si>
   <si>
-    <t>Filler2</t>
+    <t>Filler3</t>
   </si>
   <si>
     <t xml:space="preserve">Rang de naissance  </t>
@@ -621,7 +624,7 @@
     <t>DTSORT2</t>
   </si>
   <si>
-    <t>Filler3</t>
+    <t>Filler4</t>
   </si>
   <si>
     <t xml:space="preserve">Empreinte numérique </t>
@@ -641,12 +644,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,17 +663,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -682,18 +686,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -706,17 +703,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -735,30 +753,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,6 +776,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -780,32 +800,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,7 +816,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,19 +870,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,7 +900,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,7 +960,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,85 +978,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,30 +1000,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1011,6 +1007,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1023,47 +1034,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1086,176 +1063,195 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1605,11 +1601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5733333333333" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1640,7 +1636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" hidden="1" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1660,7 +1656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" hidden="1" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1680,7 +1676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" hidden="1" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1700,7 +1696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" hidden="1" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1720,7 +1716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" hidden="1" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1740,7 +1736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" hidden="1" spans="1:6">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1760,7 +1756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" hidden="1" spans="1:6">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1780,7 +1776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" hidden="1" spans="1:6">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1800,7 +1796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" hidden="1" spans="1:6">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1820,7 +1816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" hidden="1" spans="1:6">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1840,7 +1836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" hidden="1" spans="1:6">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1860,7 +1856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" hidden="1" spans="1:6">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1880,7 +1876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" hidden="1" spans="1:6">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1900,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" hidden="1" spans="1:6">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1920,7 +1916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" hidden="1" spans="1:6">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" hidden="1" spans="1:6">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1960,7 +1956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" hidden="1" spans="1:6">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" hidden="1" spans="1:6">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2000,7 +1996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" hidden="1" spans="1:6">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -2020,7 +2016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" hidden="1" spans="1:6">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2040,7 +2036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" hidden="1" spans="1:6">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" hidden="1" spans="1:6">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2080,7 +2076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" hidden="1" spans="1:6">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2100,7 +2096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" hidden="1" spans="1:6">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2120,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" hidden="1" spans="1:6">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2140,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" ht="18" customHeight="1" spans="1:6">
+    <row r="27" ht="18" hidden="1" customHeight="1" spans="1:6">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -2160,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" hidden="1" spans="1:6">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2180,7 +2176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" hidden="1" spans="1:6">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2200,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" hidden="1" spans="1:6">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2220,7 +2216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" hidden="1" spans="1:6">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2240,7 +2236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" hidden="1" spans="1:6">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -2260,7 +2256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" hidden="1" spans="1:6">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2280,7 +2276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" hidden="1" spans="1:6">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2300,7 +2296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" hidden="1" spans="1:6">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -2320,7 +2316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" hidden="1" spans="1:6">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2340,7 +2336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" hidden="1" spans="1:6">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2360,7 +2356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" hidden="1" spans="1:6">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -2400,7 +2396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" hidden="1" spans="1:6">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" hidden="1" spans="1:6">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2440,7 +2436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" hidden="1" spans="1:6">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2460,7 +2456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" hidden="1" spans="1:6">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2480,7 +2476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" hidden="1" spans="1:6">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -2500,7 +2496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" hidden="1" spans="1:6">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2520,7 +2516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" hidden="1" spans="1:6">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -2540,7 +2536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" hidden="1" spans="1:6">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -2560,7 +2556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" hidden="1" spans="1:6">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -2580,7 +2576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" hidden="1" spans="1:6">
       <c r="A49" t="s">
         <v>102</v>
       </c>
@@ -2600,7 +2596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" hidden="1" spans="1:6">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -2620,7 +2616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" hidden="1" spans="1:6">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -2640,7 +2636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" hidden="1" spans="1:6">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -2660,7 +2656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" hidden="1" spans="1:6">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -2680,7 +2676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" hidden="1" spans="1:6">
       <c r="A54" t="s">
         <v>112</v>
       </c>
@@ -2700,7 +2696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" hidden="1" spans="1:6">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -2720,7 +2716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" hidden="1" spans="1:6">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -2740,7 +2736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" hidden="1" spans="1:6">
       <c r="A57" t="s">
         <v>118</v>
       </c>
@@ -2760,7 +2756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" hidden="1" spans="1:6">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -2780,7 +2776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" hidden="1" spans="1:6">
       <c r="A59" t="s">
         <v>122</v>
       </c>
@@ -2800,7 +2796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" hidden="1" spans="1:6">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -2820,7 +2816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" hidden="1" spans="1:6">
       <c r="A61" t="s">
         <v>126</v>
       </c>
@@ -2840,7 +2836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" hidden="1" spans="1:6">
       <c r="A62" t="s">
         <v>128</v>
       </c>
@@ -2860,7 +2856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" hidden="1" spans="1:6">
       <c r="A63" t="s">
         <v>130</v>
       </c>
@@ -2880,7 +2876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" hidden="1" spans="1:6">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" hidden="1" spans="1:6">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -2920,7 +2916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" hidden="1" spans="1:6">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -2940,7 +2936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" hidden="1" spans="1:6">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -2960,7 +2956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" hidden="1" spans="1:6">
       <c r="A68" t="s">
         <v>140</v>
       </c>
@@ -2980,7 +2976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" hidden="1" spans="1:6">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -3000,7 +2996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" hidden="1" spans="1:6">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -3020,7 +3016,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" hidden="1" spans="1:6">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -3040,7 +3036,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" hidden="1" spans="1:6">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -3060,7 +3056,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" hidden="1" spans="1:6">
       <c r="A73" t="s">
         <v>151</v>
       </c>
@@ -3080,7 +3076,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" hidden="1" spans="1:6">
       <c r="A74" t="s">
         <v>153</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" hidden="1" spans="1:6">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -3120,7 +3116,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" hidden="1" spans="1:6">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -3140,7 +3136,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" hidden="1" spans="1:6">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -3180,7 +3176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" hidden="1" spans="1:6">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -3200,7 +3196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" hidden="1" spans="1:6">
       <c r="A80" t="s">
         <v>164</v>
       </c>
@@ -3220,7 +3216,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" hidden="1" spans="1:6">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -3240,7 +3236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" hidden="1" spans="1:6">
       <c r="A82" t="s">
         <v>168</v>
       </c>
@@ -3280,7 +3276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" hidden="1" spans="1:6">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -3300,7 +3296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" hidden="1" spans="1:6">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -3320,7 +3316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" hidden="1" spans="1:6">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -3340,7 +3336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" hidden="1" spans="1:6">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3360,7 +3356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" hidden="1" spans="1:6">
       <c r="A88" t="s">
         <v>179</v>
       </c>
@@ -3380,7 +3376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" hidden="1" spans="1:6">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -3400,7 +3396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" hidden="1" spans="1:6">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -3420,7 +3416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" hidden="1" spans="1:6">
       <c r="A91" t="s">
         <v>185</v>
       </c>
@@ -3440,7 +3436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" hidden="1" spans="1:6">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -3460,7 +3456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" hidden="1" spans="1:6">
       <c r="A93" t="s">
         <v>189</v>
       </c>
@@ -3480,7 +3476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" hidden="1" spans="1:6">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -3500,7 +3496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" hidden="1" spans="1:6">
       <c r="A95" t="s">
         <v>193</v>
       </c>
@@ -3520,7 +3516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" hidden="1" spans="1:6">
       <c r="A96" t="s">
         <v>195</v>
       </c>
@@ -3540,7 +3536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" hidden="1" spans="1:6">
       <c r="A97" t="s">
         <v>197</v>
       </c>
@@ -3560,7 +3556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" hidden="1" spans="1:6">
       <c r="A98" t="s">
         <v>199</v>
       </c>
@@ -3600,7 +3596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" hidden="1" spans="1:6">
       <c r="A100" t="s">
         <v>202</v>
       </c>
@@ -3620,7 +3616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" hidden="1" spans="1:6">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -3641,6 +3637,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F101">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Filler1"/>
+        <filter val="FILLER2"/>
+        <filter val="Filler3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>